<commit_message>
Updated AdminUserPage, AdminUsersTest script
</commit_message>
<xml_diff>
--- a/GroceryApplicationProject/src/test/resources/TestData.xlsx
+++ b/GroceryApplicationProject/src/test/resources/TestData.xlsx
@@ -34,7 +34,7 @@
     <t>secret_sauce</t>
   </si>
   <si>
-    <t>Glen</t>
+    <t>glen</t>
   </si>
   <si>
     <t>Admin</t>
@@ -659,6 +659,9 @@
         <v>5</v>
       </c>
       <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
created ManageNewsPage and MangeNewsTest
</commit_message>
<xml_diff>
--- a/GroceryApplicationProject/src/test/resources/TestData.xlsx
+++ b/GroceryApplicationProject/src/test/resources/TestData.xlsx
@@ -3,11 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPage" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="AdminPage" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="ManageNews" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr/>
   <extLst>
@@ -17,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>admin</t>
   </si>
@@ -38,6 +39,9 @@
   </si>
   <si>
     <t>Admin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">News Update - Glen</t>
   </si>
 </sst>
 </file>
@@ -671,4 +675,29 @@
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+  <sheetViews>
+    <sheetView zoomScale="100" workbookViewId="0">
+      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="23.421875"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>